<commit_message>
change bouwland, productief, cultivated to eco8, eco9, and eco10
</commit_message>
<xml_diff>
--- a/dev/ER_puntenregeling_aan_te_vullen_220706.xlsx
+++ b/dev/ER_puntenregeling_aan_te_vullen_220706.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ROSG\0000.N.22. nmi packages\BedrijfsBodemWaterPlanCalculator\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C82C70C-25A6-43DB-8023-4A6D4F3BA711}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68B0F05D-E222-4BC0-B350-D24FDFA03958}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CD0B0C30-B023-4E8E-BE3B-BF904258CDBD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{CD0B0C30-B023-4E8E-BE3B-BF904258CDBD}"/>
   </bookViews>
   <sheets>
     <sheet name="220706_fulldb_v6" sheetId="10" r:id="rId1"/>
@@ -2873,7 +2873,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2967,12 +2967,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="10">
@@ -3590,9 +3584,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00390964-7CCF-4BFE-AA8E-BCB0A93F871B}">
   <dimension ref="A1:CC167"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="BN1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="CM7" sqref="CM7"/>
+      <selection pane="bottomLeft" activeCell="BR1" sqref="BR1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3600,21 +3594,20 @@
     <col min="1" max="1" width="12" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
     <col min="4" max="4" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="65.7109375" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="41.140625" hidden="1" customWidth="1"/>
-    <col min="7" max="8" width="9.140625" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="21.28515625" hidden="1" customWidth="1"/>
-    <col min="10" max="38" width="9.140625" hidden="1" customWidth="1"/>
-    <col min="39" max="47" width="7.140625" hidden="1" customWidth="1"/>
-    <col min="48" max="54" width="8.140625" hidden="1" customWidth="1"/>
-    <col min="55" max="56" width="9.140625" hidden="1" customWidth="1"/>
-    <col min="57" max="57" width="8" hidden="1" customWidth="1"/>
-    <col min="58" max="58" width="9.140625" hidden="1" customWidth="1"/>
-    <col min="59" max="59" width="8" hidden="1" customWidth="1"/>
-    <col min="60" max="63" width="9.140625" hidden="1" customWidth="1"/>
-    <col min="64" max="67" width="8" hidden="1" customWidth="1"/>
-    <col min="68" max="76" width="9.140625" hidden="1" customWidth="1"/>
-    <col min="77" max="80" width="9.140625" customWidth="1"/>
+    <col min="5" max="5" width="65.7109375" customWidth="1"/>
+    <col min="6" max="6" width="41.140625" customWidth="1"/>
+    <col min="7" max="8" width="9.140625" customWidth="1"/>
+    <col min="9" max="9" width="21.28515625" customWidth="1"/>
+    <col min="10" max="38" width="9.140625" customWidth="1"/>
+    <col min="39" max="47" width="7.140625" customWidth="1"/>
+    <col min="48" max="54" width="8.140625" customWidth="1"/>
+    <col min="55" max="56" width="9.140625" customWidth="1"/>
+    <col min="57" max="57" width="8" customWidth="1"/>
+    <col min="58" max="58" width="9.140625" customWidth="1"/>
+    <col min="59" max="59" width="8" customWidth="1"/>
+    <col min="60" max="63" width="9.140625" customWidth="1"/>
+    <col min="64" max="67" width="8" customWidth="1"/>
+    <col min="68" max="80" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:81" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -94425,6 +94418,27 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="4cc40f53-1c4d-406e-8b7f-b0d2efc65169" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="390f5cb6-d64a-4bc2-898f-27f28368359d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <_DCDateCreated xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005D9EB5DCBC0D6E41AA26ADC096BADFA2" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="eaee64eac79edd06b78e709dea506ce8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="390f5cb6-d64a-4bc2-898f-27f28368359d" xmlns:ns3="http://schemas.microsoft.com/sharepoint/v3/fields" xmlns:ns4="4cc40f53-1c4d-406e-8b7f-b0d2efc65169" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5977707cf50c60c2b0ea4422a86d8247" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="390f5cb6-d64a-4bc2-898f-27f28368359d"/>
@@ -94678,43 +94692,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="4cc40f53-1c4d-406e-8b7f-b0d2efc65169" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="390f5cb6-d64a-4bc2-898f-27f28368359d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <_DCDateCreated xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3B7A3F09-833A-4435-8766-0EE291EB583A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E652E760-0C03-45C4-9B4D-D57055B6C3FB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="390f5cb6-d64a-4bc2-898f-27f28368359d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
-    <ds:schemaRef ds:uri="4cc40f53-1c4d-406e-8b7f-b0d2efc65169"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -94738,9 +94719,21 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E652E760-0C03-45C4-9B4D-D57055B6C3FB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3B7A3F09-833A-4435-8766-0EE291EB583A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="390f5cb6-d64a-4bc2-898f-27f28368359d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
+    <ds:schemaRef ds:uri="4cc40f53-1c4d-406e-8b7f-b0d2efc65169"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
fix duplicated bbwp_id in measures
</commit_message>
<xml_diff>
--- a/dev/ER_puntenregeling_aan_te_vullen_220706.xlsx
+++ b/dev/ER_puntenregeling_aan_te_vullen_220706.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ROSG\0000.N.22. nmi packages\BedrijfsBodemWaterPlanCalculator\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68B0F05D-E222-4BC0-B350-D24FDFA03958}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDD7C430-71FB-4E2D-BD84-2ADFB7761870}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{CD0B0C30-B023-4E8E-BE3B-BF904258CDBD}"/>
   </bookViews>
@@ -407,7 +407,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3896" uniqueCount="819">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3896" uniqueCount="821">
   <si>
     <t>bbwp_id</t>
   </si>
@@ -2868,6 +2868,12 @@
   <si>
     <t>acc_glmc</t>
   </si>
+  <si>
+    <t>B192</t>
+  </si>
+  <si>
+    <t>EG13</t>
+  </si>
 </sst>
 </file>
 
@@ -3584,9 +3590,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00390964-7CCF-4BFE-AA8E-BCB0A93F871B}">
   <dimension ref="A1:CC167"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BN1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="BR1" sqref="BR1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11555,8 +11561,8 @@
       <c r="C41">
         <v>62</v>
       </c>
-      <c r="D41" s="2" t="s">
-        <v>417</v>
+      <c r="D41" s="46" t="s">
+        <v>820</v>
       </c>
       <c r="E41" s="46" t="s">
         <v>466</v>
@@ -12707,8 +12713,8 @@
       </c>
     </row>
     <row r="47" spans="1:81" x14ac:dyDescent="0.25">
-      <c r="A47" s="49" t="s">
-        <v>173</v>
+      <c r="A47" s="46" t="s">
+        <v>819</v>
       </c>
       <c r="C47">
         <v>34</v>
@@ -36679,9 +36685,9 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:CI179"/>
   <sheetViews>
-    <sheetView topLeftCell="AW1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A82" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="BP180" sqref="BP180"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E76" sqref="E76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -36689,17 +36695,20 @@
     <col min="1" max="1" width="12" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
     <col min="4" max="4" width="14.7109375" customWidth="1"/>
-    <col min="5" max="5" width="96.7109375" customWidth="1"/>
+    <col min="5" max="5" width="29.7109375" customWidth="1"/>
     <col min="6" max="6" width="17.85546875" customWidth="1"/>
     <col min="7" max="8" width="9.140625" customWidth="1"/>
     <col min="9" max="9" width="21.28515625" customWidth="1"/>
-    <col min="10" max="38" width="9.140625" customWidth="1"/>
-    <col min="39" max="47" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="48" max="49" width="8.140625" customWidth="1"/>
-    <col min="50" max="54" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="8" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="8" bestFit="1" customWidth="1"/>
-    <col min="64" max="67" width="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="38" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="39" max="47" width="7.140625" hidden="1" customWidth="1"/>
+    <col min="48" max="54" width="8.140625" hidden="1" customWidth="1"/>
+    <col min="55" max="56" width="0" hidden="1" customWidth="1"/>
+    <col min="57" max="57" width="8" hidden="1" customWidth="1"/>
+    <col min="58" max="58" width="0" hidden="1" customWidth="1"/>
+    <col min="59" max="59" width="8" hidden="1" customWidth="1"/>
+    <col min="60" max="63" width="0" hidden="1" customWidth="1"/>
+    <col min="64" max="67" width="8" hidden="1" customWidth="1"/>
+    <col min="68" max="70" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:83" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -37757,7 +37766,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="7" spans="1:83" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>173</v>
       </c>
@@ -37932,7 +37941,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="8" spans="1:83" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>173</v>
       </c>
@@ -39244,7 +39253,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="1:84" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>177</v>
       </c>
@@ -39416,7 +39425,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="18" spans="1:84" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>45</v>
       </c>
@@ -39591,7 +39600,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="19" spans="1:84" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>51</v>
       </c>
@@ -39763,7 +39772,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="20" spans="1:84" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>54</v>
       </c>
@@ -39935,7 +39944,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="21" spans="1:84" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>57</v>
       </c>
@@ -40107,7 +40116,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="22" spans="1:84" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>60</v>
       </c>
@@ -40279,7 +40288,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="23" spans="1:84" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>64</v>
       </c>
@@ -40451,7 +40460,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="24" spans="1:84" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>68</v>
       </c>
@@ -40626,7 +40635,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="25" spans="1:84" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>71</v>
       </c>
@@ -40801,7 +40810,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="26" spans="1:84" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>74</v>
       </c>
@@ -40973,7 +40982,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="27" spans="1:84" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>77</v>
       </c>
@@ -41145,7 +41154,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="28" spans="1:84" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>80</v>
       </c>
@@ -41317,7 +41326,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="29" spans="1:84" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>83</v>
       </c>
@@ -42177,7 +42186,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="34" spans="1:84" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>105</v>
       </c>
@@ -42416,7 +42425,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="35" spans="1:84" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>108</v>
       </c>
@@ -42655,7 +42664,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="36" spans="1:84" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>111</v>
       </c>
@@ -42827,7 +42836,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="37" spans="1:84" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>114</v>
       </c>
@@ -42999,7 +43008,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="38" spans="1:84" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>117</v>
       </c>
@@ -43171,7 +43180,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="39" spans="1:84" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>120</v>
       </c>
@@ -43343,7 +43352,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="40" spans="1:84" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>164</v>
       </c>
@@ -43518,7 +43527,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="41" spans="1:84" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>167</v>
       </c>
@@ -43693,7 +43702,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="42" spans="1:84" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>170</v>
       </c>
@@ -43871,7 +43880,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="43" spans="1:84" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>186</v>
       </c>
@@ -44037,7 +44046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:84" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>186</v>
       </c>
@@ -44203,7 +44212,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:84" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>186</v>
       </c>
@@ -44369,7 +44378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:84" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>186</v>
       </c>
@@ -44535,7 +44544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:84" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>186</v>
       </c>
@@ -44701,7 +44710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:84" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>186</v>
       </c>
@@ -44867,7 +44876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:87" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>187</v>
       </c>
@@ -45033,7 +45042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:87" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>187</v>
       </c>
@@ -45199,7 +45208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:87" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>187</v>
       </c>
@@ -45365,7 +45374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:87" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>187</v>
       </c>
@@ -45531,7 +45540,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:87" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>187</v>
       </c>
@@ -45697,7 +45706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:87" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>187</v>
       </c>
@@ -45863,7 +45872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:87" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>189</v>
       </c>
@@ -46029,7 +46038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:87" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>189</v>
       </c>
@@ -46195,7 +46204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:87" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>189</v>
       </c>
@@ -46361,7 +46370,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:87" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>189</v>
       </c>
@@ -46527,7 +46536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:87" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>189</v>
       </c>
@@ -46693,7 +46702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:87" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>189</v>
       </c>
@@ -46859,7 +46868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:87" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>191</v>
       </c>
@@ -47031,7 +47040,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="62" spans="1:87" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>203</v>
       </c>
@@ -47207,7 +47216,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="63" spans="1:87" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>207</v>
       </c>
@@ -47380,7 +47389,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="64" spans="1:87" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>210</v>
       </c>
@@ -47556,7 +47565,7 @@
       <c r="CH64" s="7"/>
       <c r="CI64" s="7"/>
     </row>
-    <row r="65" spans="1:84" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>213</v>
       </c>
@@ -47726,7 +47735,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="66" spans="1:84" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>242</v>
       </c>
@@ -47904,7 +47913,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="67" spans="1:84" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>245</v>
       </c>
@@ -48082,7 +48091,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="68" spans="1:84" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>248</v>
       </c>
@@ -48260,7 +48269,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="69" spans="1:84" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>288</v>
       </c>
@@ -48432,7 +48441,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="70" spans="1:84" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>290</v>
       </c>
@@ -48604,7 +48613,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="71" spans="1:84" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>300</v>
       </c>
@@ -48770,7 +48779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:84" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>303</v>
       </c>
@@ -48939,7 +48948,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:84" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>194</v>
       </c>
@@ -49108,7 +49117,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="74" spans="1:84" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>194</v>
       </c>
@@ -49280,7 +49289,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="75" spans="1:84" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>194</v>
       </c>
@@ -49452,7 +49461,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="76" spans="1:84" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>139</v>
       </c>
@@ -49627,7 +49636,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="77" spans="1:84" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>142</v>
       </c>
@@ -49802,7 +49811,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="78" spans="1:84" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>144</v>
       </c>
@@ -50285,7 +50294,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="81" spans="1:83" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>233</v>
       </c>
@@ -50457,7 +50466,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="82" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:83" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>277</v>
       </c>
@@ -50626,7 +50635,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="83" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:83" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>277</v>
       </c>
@@ -50795,7 +50804,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="84" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:83" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>277</v>
       </c>
@@ -50964,7 +50973,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="85" spans="1:83" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>160</v>
       </c>
@@ -55506,7 +55515,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="108" spans="1:83" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>282</v>
       </c>
@@ -56960,7 +56969,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="115" spans="1:83" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>99</v>
       </c>
@@ -59420,7 +59429,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="127" spans="1:83" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>152</v>
       </c>
@@ -59656,7 +59665,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:83" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>152</v>
       </c>
@@ -60295,7 +60304,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="131" spans="1:83" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>261</v>
       </c>
@@ -60534,7 +60543,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="132" spans="1:83" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>261</v>
       </c>
@@ -60773,7 +60782,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="133" spans="1:83" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>261</v>
       </c>
@@ -61012,7 +61021,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="134" spans="1:83" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>261</v>
       </c>
@@ -61251,7 +61260,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="135" spans="1:83" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>261</v>
       </c>
@@ -61490,7 +61499,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="136" spans="1:83" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>261</v>
       </c>
@@ -62135,7 +62144,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="139" spans="1:83" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>157</v>
       </c>
@@ -62374,7 +62383,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="140" spans="1:83" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>157</v>
       </c>
@@ -62613,7 +62622,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="141" spans="1:83" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>157</v>
       </c>
@@ -62856,7 +62865,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="142" spans="1:83" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>157</v>
       </c>
@@ -63083,7 +63092,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="143" spans="1:83" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>225</v>
       </c>
@@ -63322,7 +63331,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="144" spans="1:83" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>225</v>
       </c>
@@ -63964,7 +63973,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="147" spans="1:83" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>130</v>
       </c>
@@ -64203,7 +64212,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="148" spans="1:83" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>130</v>
       </c>
@@ -64430,7 +64439,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="149" spans="1:83" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>180</v>
       </c>
@@ -64669,7 +64678,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="150" spans="1:83" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>180</v>
       </c>
@@ -64909,7 +64918,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="151" spans="1:83" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>251</v>
       </c>
@@ -65148,7 +65157,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="152" spans="1:83" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>251</v>
       </c>
@@ -65387,7 +65396,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="153" spans="1:83" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>251</v>
       </c>
@@ -65626,7 +65635,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="154" spans="1:83" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>216</v>
       </c>
@@ -65866,7 +65875,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="155" spans="1:83" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>216</v>
       </c>
@@ -67521,7 +67530,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="163" spans="1:83" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>123</v>
       </c>
@@ -70704,7 +70713,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="178" spans="1:83" hidden="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>149</v>
       </c>
@@ -70867,7 +70876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:83" hidden="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>149</v>
       </c>
@@ -71033,12 +71042,13 @@
   </sheetData>
   <autoFilter ref="A1:CI179" xr:uid="{0B97C9B8-C0CC-4A2E-A96E-6D5D6A736452}">
     <filterColumn colId="3">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
+    <filterColumn colId="7">
       <filters>
-        <filter val="EB14A"/>
-        <filter val="EB14B"/>
-        <filter val="EB14C"/>
-        <filter val="EG14A"/>
-        <filter val="EG14B"/>
+        <filter val="field"/>
       </filters>
     </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:CI179">
@@ -94418,27 +94428,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="4cc40f53-1c4d-406e-8b7f-b0d2efc65169" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="390f5cb6-d64a-4bc2-898f-27f28368359d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <_DCDateCreated xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005D9EB5DCBC0D6E41AA26ADC096BADFA2" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="eaee64eac79edd06b78e709dea506ce8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="390f5cb6-d64a-4bc2-898f-27f28368359d" xmlns:ns3="http://schemas.microsoft.com/sharepoint/v3/fields" xmlns:ns4="4cc40f53-1c4d-406e-8b7f-b0d2efc65169" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5977707cf50c60c2b0ea4422a86d8247" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="390f5cb6-d64a-4bc2-898f-27f28368359d"/>
@@ -94692,10 +94681,43 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="4cc40f53-1c4d-406e-8b7f-b0d2efc65169" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="390f5cb6-d64a-4bc2-898f-27f28368359d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <_DCDateCreated xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E652E760-0C03-45C4-9B4D-D57055B6C3FB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3B7A3F09-833A-4435-8766-0EE291EB583A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="390f5cb6-d64a-4bc2-898f-27f28368359d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
+    <ds:schemaRef ds:uri="4cc40f53-1c4d-406e-8b7f-b0d2efc65169"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -94719,21 +94741,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3B7A3F09-833A-4435-8766-0EE291EB583A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E652E760-0C03-45C4-9B4D-D57055B6C3FB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="390f5cb6-d64a-4bc2-898f-27f28368359d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
-    <ds:schemaRef ds:uri="4cc40f53-1c4d-406e-8b7f-b0d2efc65169"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>